<commit_message>
modified:   maneuvers/maneuver1.xlsx 	modified:   maneuvers/maneuver3.xlsx
</commit_message>
<xml_diff>
--- a/maneuvers/maneuver1.xlsx
+++ b/maneuvers/maneuver1.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\HiroyoshiH\Documents\EngProjects\PPJ1900153_Ohtake_WFM\workspace\trial_repo\maneuvers\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\HiroyoshiH\Documents\EngProjects\PPJ1900153_Ohtake_WFM\workspace\test\trial_repo\maneuvers\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C9E2A7B3-FB6B-4971-92D1-9D771ABAF679}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BE25F96C-A31F-4531-A811-52BEFF107461}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="2856" yWindow="1920" windowWidth="16584" windowHeight="9420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1" uniqueCount="1">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="1">
   <si>
     <t>change added</t>
     <phoneticPr fontId="1"/>
@@ -353,10 +353,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1"/>
+  <dimension ref="A1:A2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G7" sqref="G7"/>
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18"/>
@@ -366,6 +366,11 @@
         <v>0</v>
       </c>
     </row>
+    <row r="2" spans="1:1">
+      <c r="A2" t="s">
+        <v>0</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>